<commit_message>
similar to emph table
</commit_message>
<xml_diff>
--- a/demographics_BMI_statistics.xlsx
+++ b/demographics_BMI_statistics.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
-  <si>
-    <t>All participants</t>
-  </si>
-  <si>
-    <t>Participants with low BMI</t>
-  </si>
-  <si>
-    <t>Participants with high BMI</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>All participants (N=358)</t>
+  </si>
+  <si>
+    <t>Participants with low BMI (N=178)</t>
+  </si>
+  <si>
+    <t>Participants with high BMI (N=180)</t>
   </si>
   <si>
     <t>P value</t>
@@ -31,13 +31,7 @@
     <t>Characteristics</t>
   </si>
   <si>
-    <t>Number of participants</t>
-  </si>
-  <si>
-    <t>Gender Male</t>
-  </si>
-  <si>
-    <t>Gender Female</t>
+    <t>Sex (male, %)</t>
   </si>
   <si>
     <t>Age</t>
@@ -58,37 +52,28 @@
     <t>Pack years</t>
   </si>
   <si>
-    <t>68 (19.0%)</t>
-  </si>
-  <si>
-    <t>292 (81.0%)</t>
+    <t>67 (19.0%)</t>
   </si>
   <si>
     <t>59.8±10.3</t>
   </si>
   <si>
-    <t>85.7±32.9</t>
-  </si>
-  <si>
-    <t>170.9±8.5</t>
-  </si>
-  <si>
-    <t>138 (38.0%)</t>
-  </si>
-  <si>
-    <t>191 (53.0%)</t>
-  </si>
-  <si>
-    <t>15.1±14.1</t>
-  </si>
-  <si>
-    <t>180 (50.0%)</t>
-  </si>
-  <si>
-    <t>25 (13.9%)</t>
-  </si>
-  <si>
-    <t>155 (86.1%)</t>
+    <t>85.9±32.9</t>
+  </si>
+  <si>
+    <t>170.9±8.6</t>
+  </si>
+  <si>
+    <t>138 (39.0%)</t>
+  </si>
+  <si>
+    <t>189 (53.0%)</t>
+  </si>
+  <si>
+    <t>15.1±14.2</t>
+  </si>
+  <si>
+    <t>24 (13.5%)</t>
   </si>
   <si>
     <t>61.3±10.8</t>
@@ -100,19 +85,16 @@
     <t>171.2±8.3</t>
   </si>
   <si>
-    <t>82 (45.6%)</t>
-  </si>
-  <si>
-    <t>89 (49.4%)</t>
-  </si>
-  <si>
-    <t>15.1±13.1</t>
+    <t>82 (46.1%)</t>
+  </si>
+  <si>
+    <t>87 (48.9%)</t>
+  </si>
+  <si>
+    <t>15.2±13.2</t>
   </si>
   <si>
     <t>43 (24.0%)</t>
-  </si>
-  <si>
-    <t>137 (76.0%)</t>
   </si>
   <si>
     <t>58.2±9.5</t>
@@ -491,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,14 +500,17 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>360</v>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>0.017</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -533,16 +518,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>0.022</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -550,13 +535,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -564,16 +552,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E5">
-        <v>0.004</v>
+        <v>0.534</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -581,16 +569,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>0.023</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -598,16 +586,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7">
-        <v>0.531</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -615,47 +600,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8">
-        <v>0.029</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10">
-        <v>0.96</v>
+        <v>0.947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>